<commit_message>
Solução: MP Versão: 1.0 Msg: Continuação do desenvolvendo da tela de TipoDePatente.
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Chrisley.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Chrisley.xlsx
@@ -27,12 +27,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="DD/MM/YY" numFmtId="165"/>
+    <numFmt formatCode="HH:MM:SS" numFmtId="166"/>
   </numFmts>
   <fonts count="4">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -94,8 +97,16 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -116,10 +127,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B11" activeCellId="0" pane="topLeft" sqref="B11"/>
+      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -129,12 +140,20 @@
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="2">
+      <c r="A2" s="1" t="n">
+        <v>41548</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0.0833333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>